<commit_message>
version final para 2da entrega
</commit_message>
<xml_diff>
--- a/myJSON/ejemploexcel.xlsx
+++ b/myJSON/ejemploexcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\$_CoderHouse\Desarrollo Web\Clase 11\Viziozone 11\myJSON\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F954B4-1E4F-4906-9347-3FD4552E44B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61A8F2B-6453-4F18-90AE-0B30385048E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{20F415A7-21AA-4A3F-AD72-4D8403B98674}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="519">
   <si>
     <t>PROCESADOR</t>
   </si>
@@ -1462,13 +1462,133 @@
   </si>
   <si>
     <t>Almacen</t>
+  </si>
+  <si>
+    <t>RYZEN</t>
+  </si>
+  <si>
+    <t>3200G</t>
+  </si>
+  <si>
+    <t>3300X</t>
+  </si>
+  <si>
+    <t>3400G</t>
+  </si>
+  <si>
+    <t>2600X</t>
+  </si>
+  <si>
+    <t>3500X</t>
+  </si>
+  <si>
+    <t>3600X</t>
+  </si>
+  <si>
+    <t>5600X</t>
+  </si>
+  <si>
+    <t>3700X</t>
+  </si>
+  <si>
+    <t>3800X</t>
+  </si>
+  <si>
+    <t>3800XT</t>
+  </si>
+  <si>
+    <t>5800X</t>
+  </si>
+  <si>
+    <t>3900X</t>
+  </si>
+  <si>
+    <t>5900X</t>
+  </si>
+  <si>
+    <t>3950X</t>
+  </si>
+  <si>
+    <t>5950X</t>
+  </si>
+  <si>
+    <t>THREADRIPPER</t>
+  </si>
+  <si>
+    <t>3960X</t>
+  </si>
+  <si>
+    <t>3970X</t>
+  </si>
+  <si>
+    <t>CORE</t>
+  </si>
+  <si>
+    <t>I3</t>
+  </si>
+  <si>
+    <t>9100F</t>
+  </si>
+  <si>
+    <t>PENTIUM</t>
+  </si>
+  <si>
+    <t>GOLD</t>
+  </si>
+  <si>
+    <t>G5400,</t>
+  </si>
+  <si>
+    <t>10100F</t>
+  </si>
+  <si>
+    <t>I5</t>
+  </si>
+  <si>
+    <t>9400F</t>
+  </si>
+  <si>
+    <t>10400F</t>
+  </si>
+  <si>
+    <t>9600K</t>
+  </si>
+  <si>
+    <t>10600K</t>
+  </si>
+  <si>
+    <t>I7</t>
+  </si>
+  <si>
+    <t>9700K</t>
+  </si>
+  <si>
+    <t>10700F</t>
+  </si>
+  <si>
+    <t>10700K</t>
+  </si>
+  <si>
+    <t>I9</t>
+  </si>
+  <si>
+    <t>9900KF</t>
+  </si>
+  <si>
+    <t>10850K</t>
+  </si>
+  <si>
+    <t>10900KF</t>
+  </si>
+  <si>
+    <t>10900K</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1488,6 +1608,21 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1519,10 +1654,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1837,19 +1976,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52E59464-E206-4C05-9F47-FA33144B9F1E}">
-  <dimension ref="A2:G209"/>
+  <dimension ref="A2:Q209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+      <selection activeCell="P164" sqref="P164:P169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="87.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="52.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>465</v>
       </c>
@@ -1872,7 +2013,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -1891,8 +2032,30 @@
       <c r="G3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="L3" s="3">
+        <v>3</v>
+      </c>
+      <c r="M3" s="3">
+        <v>3100</v>
+      </c>
+      <c r="N3" s="3"/>
+      <c r="O3" s="4" t="str">
+        <f>_xlfn.CONCAT(J3&amp;" "&amp;K3&amp;" "&amp;L3&amp;" "&amp;M3)</f>
+        <v>AMD RYZEN 3 3100</v>
+      </c>
+      <c r="P3" s="5" t="str">
+        <f>"'"&amp;O3&amp;"',"</f>
+        <v>'AMD RYZEN 3 3100',</v>
+      </c>
+      <c r="Q3" s="6"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -1911,8 +2074,30 @@
       <c r="G4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="L4" s="3">
+        <v>3</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="N4" s="3"/>
+      <c r="O4" s="4" t="str">
+        <f t="shared" ref="O4:O40" si="0">_xlfn.CONCAT(J4&amp;" "&amp;K4&amp;" "&amp;L4&amp;" "&amp;M4)</f>
+        <v>AMD RYZEN 3 3200G</v>
+      </c>
+      <c r="P4" s="5" t="str">
+        <f t="shared" ref="P4:P20" si="1">"'"&amp;O4&amp;"',"</f>
+        <v>'AMD RYZEN 3 3200G',</v>
+      </c>
+      <c r="Q4" s="6"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -1931,8 +2116,30 @@
       <c r="G5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="L5" s="3">
+        <v>3</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="N5" s="3"/>
+      <c r="O5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>AMD RYZEN 3 3300X</v>
+      </c>
+      <c r="P5" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>'AMD RYZEN 3 3300X',</v>
+      </c>
+      <c r="Q5" s="6"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>0</v>
       </c>
@@ -1951,8 +2158,30 @@
       <c r="G6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="L6" s="3">
+        <v>5</v>
+      </c>
+      <c r="M6" s="3">
+        <v>2600</v>
+      </c>
+      <c r="N6" s="3"/>
+      <c r="O6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>AMD RYZEN 5 2600</v>
+      </c>
+      <c r="P6" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>'AMD RYZEN 5 2600',</v>
+      </c>
+      <c r="Q6" s="6"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>0</v>
       </c>
@@ -1971,8 +2200,30 @@
       <c r="G7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="L7" s="3">
+        <v>5</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="N7" s="3"/>
+      <c r="O7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>AMD RYZEN 5 3400G</v>
+      </c>
+      <c r="P7" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>'AMD RYZEN 5 3400G',</v>
+      </c>
+      <c r="Q7" s="6"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>0</v>
       </c>
@@ -1991,8 +2242,30 @@
       <c r="G8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="L8" s="3">
+        <v>5</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="N8" s="3"/>
+      <c r="O8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>AMD RYZEN 5 2600X</v>
+      </c>
+      <c r="P8" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>'AMD RYZEN 5 2600X',</v>
+      </c>
+      <c r="Q8" s="6"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>0</v>
       </c>
@@ -2011,8 +2284,30 @@
       <c r="G9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="L9" s="3">
+        <v>5</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="N9" s="3"/>
+      <c r="O9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>AMD RYZEN 5 3500X</v>
+      </c>
+      <c r="P9" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>'AMD RYZEN 5 3500X',</v>
+      </c>
+      <c r="Q9" s="6"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>0</v>
       </c>
@@ -2031,8 +2326,30 @@
       <c r="G10" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="L10" s="3">
+        <v>5</v>
+      </c>
+      <c r="M10" s="3">
+        <v>3600</v>
+      </c>
+      <c r="N10" s="3"/>
+      <c r="O10" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>AMD RYZEN 5 3600</v>
+      </c>
+      <c r="P10" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>'AMD RYZEN 5 3600',</v>
+      </c>
+      <c r="Q10" s="6"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>0</v>
       </c>
@@ -2051,8 +2368,30 @@
       <c r="G11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="L11" s="3">
+        <v>5</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="N11" s="3"/>
+      <c r="O11" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>AMD RYZEN 5 3600X</v>
+      </c>
+      <c r="P11" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>'AMD RYZEN 5 3600X',</v>
+      </c>
+      <c r="Q11" s="6"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>0</v>
       </c>
@@ -2071,8 +2410,30 @@
       <c r="G12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="L12" s="3">
+        <v>5</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="N12" s="3"/>
+      <c r="O12" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>AMD RYZEN 5 5600X</v>
+      </c>
+      <c r="P12" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>'AMD RYZEN 5 5600X',</v>
+      </c>
+      <c r="Q12" s="6"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>0</v>
       </c>
@@ -2091,8 +2452,30 @@
       <c r="G13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="L13" s="3">
+        <v>7</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="N13" s="3"/>
+      <c r="O13" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>AMD RYZEN 7 3700X</v>
+      </c>
+      <c r="P13" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>'AMD RYZEN 7 3700X',</v>
+      </c>
+      <c r="Q13" s="6"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>0</v>
       </c>
@@ -2111,8 +2494,30 @@
       <c r="G14" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="L14" s="3">
+        <v>7</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="N14" s="3"/>
+      <c r="O14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>AMD RYZEN 7 3800X</v>
+      </c>
+      <c r="P14" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>'AMD RYZEN 7 3800X',</v>
+      </c>
+      <c r="Q14" s="6"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>0</v>
       </c>
@@ -2131,8 +2536,30 @@
       <c r="G15" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="L15" s="3">
+        <v>7</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="N15" s="3"/>
+      <c r="O15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>AMD RYZEN 7 3800XT</v>
+      </c>
+      <c r="P15" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>'AMD RYZEN 7 3800XT',</v>
+      </c>
+      <c r="Q15" s="6"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>0</v>
       </c>
@@ -2151,8 +2578,30 @@
       <c r="G16" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="L16" s="3">
+        <v>7</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="N16" s="3"/>
+      <c r="O16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>AMD RYZEN 7 5800X</v>
+      </c>
+      <c r="P16" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>'AMD RYZEN 7 5800X',</v>
+      </c>
+      <c r="Q16" s="6"/>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>0</v>
       </c>
@@ -2171,8 +2620,30 @@
       <c r="G17" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="L17" s="3">
+        <v>9</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="N17" s="3"/>
+      <c r="O17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>AMD RYZEN 9 3900X</v>
+      </c>
+      <c r="P17" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>'AMD RYZEN 9 3900X',</v>
+      </c>
+      <c r="Q17" s="6"/>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>0</v>
       </c>
@@ -2191,8 +2662,30 @@
       <c r="G18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="L18" s="3">
+        <v>9</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="N18" s="3"/>
+      <c r="O18" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>AMD RYZEN 9 5900X</v>
+      </c>
+      <c r="P18" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>'AMD RYZEN 9 5900X',</v>
+      </c>
+      <c r="Q18" s="6"/>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>0</v>
       </c>
@@ -2211,8 +2704,30 @@
       <c r="G19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="L19" s="3">
+        <v>9</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="N19" s="3"/>
+      <c r="O19" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>AMD RYZEN 9 3950X</v>
+      </c>
+      <c r="P19" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>'AMD RYZEN 9 3950X',</v>
+      </c>
+      <c r="Q19" s="6"/>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>0</v>
       </c>
@@ -2231,8 +2746,30 @@
       <c r="G20" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="L20" s="3">
+        <v>9</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="N20" s="3"/>
+      <c r="O20" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>AMD RYZEN 9 5950X</v>
+      </c>
+      <c r="P20" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>'AMD RYZEN 9 5950X',</v>
+      </c>
+      <c r="Q20" s="6"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>0</v>
       </c>
@@ -2251,8 +2788,27 @@
       <c r="G21" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="N21" s="3"/>
+      <c r="O21" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>AMD RYZEN THREADRIPPER 3960X</v>
+      </c>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="6"/>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>0</v>
       </c>
@@ -2271,8 +2827,27 @@
       <c r="G22" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="N22" s="3"/>
+      <c r="O22" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>AMD RYZEN THREADRIPPER 3970X</v>
+      </c>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="6"/>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>0</v>
       </c>
@@ -2291,8 +2866,27 @@
       <c r="G23" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J23" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>INTEL CORE I3 9100F</v>
+      </c>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="6"/>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>0</v>
       </c>
@@ -2311,8 +2905,27 @@
       <c r="G24" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J24" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>INTEL PENTIUM GOLD G5400,</v>
+      </c>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="6"/>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>0</v>
       </c>
@@ -2331,8 +2944,27 @@
       <c r="G25" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J25" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>INTEL CORE I3 10100F</v>
+      </c>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="6"/>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>0</v>
       </c>
@@ -2351,8 +2983,27 @@
       <c r="G26" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J26" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="M26" s="3">
+        <v>10100</v>
+      </c>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>INTEL CORE I3 10100</v>
+      </c>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="6"/>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>0</v>
       </c>
@@ -2371,8 +3022,27 @@
       <c r="G27" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J27" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>INTEL CORE I5 9400F</v>
+      </c>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="6"/>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>0</v>
       </c>
@@ -2391,8 +3061,27 @@
       <c r="G28" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J28" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>INTEL CORE I5 10400F</v>
+      </c>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="6"/>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>0</v>
       </c>
@@ -2411,8 +3100,27 @@
       <c r="G29" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J29" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="M29" s="3">
+        <v>10400</v>
+      </c>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>INTEL CORE I5 10400</v>
+      </c>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="6"/>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>0</v>
       </c>
@@ -2431,8 +3139,27 @@
       <c r="G30" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J30" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>INTEL CORE I5 9600K</v>
+      </c>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="6"/>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>0</v>
       </c>
@@ -2451,8 +3178,27 @@
       <c r="G31" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J31" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>INTEL CORE I5 10600K</v>
+      </c>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="6"/>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>0</v>
       </c>
@@ -2471,8 +3217,27 @@
       <c r="G32" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J32" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="M32" s="3">
+        <v>9700</v>
+      </c>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>INTEL CORE I7 9700</v>
+      </c>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="6"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>0</v>
       </c>
@@ -2491,8 +3256,27 @@
       <c r="G33" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J33" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="M33" s="3">
+        <v>10700</v>
+      </c>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>INTEL CORE I7 10700</v>
+      </c>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="6"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>0</v>
       </c>
@@ -2511,8 +3295,27 @@
       <c r="G34" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J34" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="M34" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>INTEL CORE I7 9700K</v>
+      </c>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="6"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>0</v>
       </c>
@@ -2531,8 +3334,27 @@
       <c r="G35" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J35" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="L35" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="M35" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>INTEL CORE I7 10700F</v>
+      </c>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="6"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>0</v>
       </c>
@@ -2551,8 +3373,27 @@
       <c r="G36" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J36" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="M36" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>INTEL CORE I7 10700K</v>
+      </c>
+      <c r="P36" s="5"/>
+      <c r="Q36" s="6"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>0</v>
       </c>
@@ -2571,8 +3412,27 @@
       <c r="G37" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J37" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="L37" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="M37" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>INTEL CORE I9 9900KF</v>
+      </c>
+      <c r="P37" s="5"/>
+      <c r="Q37" s="6"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>0</v>
       </c>
@@ -2591,8 +3451,27 @@
       <c r="G38" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J38" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="M38" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>INTEL CORE I9 10850K</v>
+      </c>
+      <c r="P38" s="5"/>
+      <c r="Q38" s="6"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>0</v>
       </c>
@@ -2611,8 +3490,27 @@
       <c r="G39" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J39" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="L39" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="M39" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>INTEL CORE I9 10900KF</v>
+      </c>
+      <c r="P39" s="5"/>
+      <c r="Q39" s="6"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>0</v>
       </c>
@@ -2631,13 +3529,32 @@
       <c r="G40" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J40" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="L40" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="M40" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>INTEL CORE I9 10900K</v>
+      </c>
+      <c r="P40" s="5"/>
+      <c r="Q40" s="6"/>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>467</v>
       </c>
@@ -2657,7 +3574,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>467</v>
       </c>
@@ -2677,7 +3594,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>467</v>
       </c>
@@ -2697,7 +3614,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>467</v>
       </c>
@@ -2717,7 +3634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>467</v>
       </c>
@@ -2737,7 +3654,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>467</v>
       </c>
@@ -3077,7 +3994,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>467</v>
       </c>
@@ -3097,7 +4014,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>467</v>
       </c>
@@ -3117,7 +4034,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>467</v>
       </c>
@@ -3137,7 +4054,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>467</v>
       </c>
@@ -3157,7 +4074,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>467</v>
       </c>
@@ -3177,7 +4094,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>467</v>
       </c>
@@ -3197,7 +4114,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>467</v>
       </c>
@@ -3217,7 +4134,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>467</v>
       </c>
@@ -3237,7 +4154,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>467</v>
       </c>
@@ -3257,7 +4174,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>467</v>
       </c>
@@ -3277,7 +4194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>467</v>
       </c>
@@ -3297,7 +4214,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>467</v>
       </c>
@@ -3317,7 +4234,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>467</v>
       </c>
@@ -3337,7 +4254,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>468</v>
       </c>
@@ -3356,8 +4273,12 @@
       <c r="G78" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P78" t="str">
+        <f>"'"&amp;D78&amp;"',"</f>
+        <v>'MB ASROCK A320M-HDV R4.0 | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="79" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>468</v>
       </c>
@@ -3376,8 +4297,12 @@
       <c r="G79" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P79" t="str">
+        <f>"'"&amp;D79&amp;"',"</f>
+        <v>'MB MSI AMD A520M-A-PRO 2 DDR44 4400MHZ HDMI DVI',</v>
+      </c>
+    </row>
+    <row r="80" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>468</v>
       </c>
@@ -3396,8 +4321,12 @@
       <c r="G80" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P80" t="str">
+        <f t="shared" ref="P80:P114" si="2">"'"&amp;D80&amp;"',"</f>
+        <v>'MB ASROCK A520M-HDV | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="81" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>468</v>
       </c>
@@ -3416,8 +4345,12 @@
       <c r="G81" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P81" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB ASROCK B450M-HDV R4.0 | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="82" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>468</v>
       </c>
@@ -3436,8 +4369,12 @@
       <c r="G82" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P82" t="str">
+        <f t="shared" si="2"/>
+        <v>'MAINBOARD GIGABYTE B450M GAMING | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="83" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>468</v>
       </c>
@@ -3456,8 +4393,12 @@
       <c r="G83" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P83" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB GIGABYTE B450M-DS3H | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="84" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>468</v>
       </c>
@@ -3476,8 +4417,12 @@
       <c r="G84" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P84" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB GIGABYTE A520M-H | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="85" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>468</v>
       </c>
@@ -3496,8 +4441,12 @@
       <c r="G85" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P85" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB GIGABYTE B450M V2 DSH3 | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="86" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>468</v>
       </c>
@@ -3516,8 +4465,12 @@
       <c r="G86" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P86" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB ASROCK B450M PRO4-F | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="87" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>468</v>
       </c>
@@ -3536,8 +4489,12 @@
       <c r="G87" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P87" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB MSI B450M PRO-M2 MAX | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="88" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>468</v>
       </c>
@@ -3556,8 +4513,12 @@
       <c r="G88" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P88" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB ASROCK B550M-HDV | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="89" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>468</v>
       </c>
@@ -3576,8 +4537,12 @@
       <c r="G89" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P89" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB ASUS PRIME B450M-A | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="90" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>468</v>
       </c>
@@ -3596,8 +4561,12 @@
       <c r="G90" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P90" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB GIGABYTE B450 AORUS M | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="91" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>468</v>
       </c>
@@ -3616,8 +4585,12 @@
       <c r="G91" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P91" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB GIGABYTE B450 AORUS ELITE | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="92" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>468</v>
       </c>
@@ -3636,8 +4609,12 @@
       <c r="G92" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P92" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB ASROCK B450 STEEL LEGEND LED- RGB | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="93" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>468</v>
       </c>
@@ -3656,8 +4633,12 @@
       <c r="G93" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P93" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB GIGABYTE B550M DS3H | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="94" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>468</v>
       </c>
@@ -3676,8 +4657,12 @@
       <c r="G94" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P94" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB ASROCK B550M PRO 4 AM4 FUTURE | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="95" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>468</v>
       </c>
@@ -3696,8 +4681,12 @@
       <c r="G95" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P95" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB ASROCK B550M PRO 4 AM4 FUTURE | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="96" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>468</v>
       </c>
@@ -3716,8 +4705,12 @@
       <c r="G96" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P96" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB ASROCK B550 PHATOM GAMING 4 (DDR4 4733+OC) | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="97" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>468</v>
       </c>
@@ -3736,8 +4729,12 @@
       <c r="G97" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P97" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB ASROCK B550 PHATOM GAMING 4/AC SOCKET AM4 (WI-FI) | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="98" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>468</v>
       </c>
@@ -3756,8 +4753,12 @@
       <c r="G98" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P98" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB B550M AORUS ELITE | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="99" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>468</v>
       </c>
@@ -3776,8 +4777,12 @@
       <c r="G99" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P99" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB ASUS TUF GAMING B550M-PLUS | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="100" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>468</v>
       </c>
@@ -3796,8 +4801,12 @@
       <c r="G100" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P100" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB ASROCK B550M STEEL LEGEND AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="101" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>468</v>
       </c>
@@ -3816,8 +4825,12 @@
       <c r="G101" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P101" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB ASUS TUF GAMING B550M-PLUS (WI-FI) | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="102" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>468</v>
       </c>
@@ -3836,8 +4849,12 @@
       <c r="G102" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P102" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB GIGABYTE X570 GAMING X | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="103" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>468</v>
       </c>
@@ -3856,8 +4873,12 @@
       <c r="G103" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P103" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB GIGABYTE B550 AORUS ELITE | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="104" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>468</v>
       </c>
@@ -3876,8 +4897,12 @@
       <c r="G104" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P104" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB ASUS ASUS PRIME X570-PRO | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="105" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>468</v>
       </c>
@@ -3896,8 +4921,12 @@
       <c r="G105" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P105" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB GIGABYTE B550 AORUS ELITE (with Dual M.2) | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="106" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>468</v>
       </c>
@@ -3916,8 +4945,12 @@
       <c r="G106" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P106" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB MSI MPG X570 GAMING PLUS | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="107" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>468</v>
       </c>
@@ -3936,8 +4969,12 @@
       <c r="G107" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P107" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB ASROCK B550 EXTREME4 | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="108" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>468</v>
       </c>
@@ -3956,8 +4993,12 @@
       <c r="G108" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P108" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB GIGABYTE B550 AORUS PRO | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="109" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>468</v>
       </c>
@@ -3976,8 +5017,12 @@
       <c r="G109" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P109" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB GIGABYTE X570 AORUS ELITE | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="110" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>468</v>
       </c>
@@ -3996,8 +5041,12 @@
       <c r="G110" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P110" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB ASUS TUF GAMING X570-PLUS WI-FI | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="111" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>468</v>
       </c>
@@ -4016,8 +5065,12 @@
       <c r="G111" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P111" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB ASUS ROG STRIX B550-E GAMING AMD RYZEN DDR4 AM4',</v>
+      </c>
+    </row>
+    <row r="112" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>468</v>
       </c>
@@ -4036,8 +5089,12 @@
       <c r="G112" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="P112" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB ASUS ROG STRIX X570-E GAMING RGB | AM4 AMD',</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>468</v>
       </c>
@@ -4056,11 +5113,15 @@
       <c r="G113" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="P113" t="str">
+        <f t="shared" si="2"/>
+        <v>'MB ASUS TUF GAMING X570-PLUS AMD RYZEN DDR4 AM4',</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D114" s="2"/>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>469</v>
       </c>
@@ -4083,7 +5144,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>470</v>
       </c>
@@ -4103,7 +5164,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>470</v>
       </c>
@@ -4123,7 +5184,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>470</v>
       </c>
@@ -4143,7 +5204,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>470</v>
       </c>
@@ -4163,7 +5224,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>470</v>
       </c>
@@ -4183,7 +5244,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>470</v>
       </c>
@@ -4203,7 +5264,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
         <v>470</v>
       </c>
@@ -4223,7 +5284,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>470</v>
       </c>
@@ -4243,7 +5304,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>470</v>
       </c>
@@ -4263,7 +5324,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>470</v>
       </c>
@@ -4283,7 +5344,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>470</v>
       </c>
@@ -4303,7 +5364,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>470</v>
       </c>
@@ -4323,7 +5384,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>470</v>
       </c>
@@ -4663,7 +5724,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="145" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
         <v>470</v>
       </c>
@@ -4683,7 +5744,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
         <v>470</v>
       </c>
@@ -4703,7 +5764,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="147" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
         <v>470</v>
       </c>
@@ -4723,7 +5784,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="148" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
         <v>470</v>
       </c>
@@ -4743,7 +5804,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="149" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
         <v>470</v>
       </c>
@@ -4763,7 +5824,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="150" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
         <v>470</v>
       </c>
@@ -4783,7 +5844,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="151" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
         <v>470</v>
       </c>
@@ -4803,7 +5864,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="152" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
         <v>470</v>
       </c>
@@ -4823,7 +5884,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="153" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
         <v>470</v>
       </c>
@@ -4843,7 +5904,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="154" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
         <v>470</v>
       </c>
@@ -4863,7 +5924,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="155" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
         <v>470</v>
       </c>
@@ -4883,7 +5944,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
         <v>470</v>
       </c>
@@ -4903,7 +5964,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="157" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
         <v>1</v>
       </c>
@@ -4923,7 +5984,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="158" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
         <v>1</v>
       </c>
@@ -4942,8 +6003,12 @@
       <c r="G158" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="159" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P158" t="str">
+        <f>"'"&amp;D158&amp;"',"</f>
+        <v>'VIEWMAX ENIGMAX RX 570 4GB',</v>
+      </c>
+    </row>
+    <row r="159" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
         <v>1</v>
       </c>
@@ -4962,8 +6027,12 @@
       <c r="G159" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="160" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P159" t="str">
+        <f t="shared" ref="P159:P170" si="3">"'"&amp;D159&amp;"',"</f>
+        <v>'VIEWMAX ENIGMAX RX 570 8GB',</v>
+      </c>
+    </row>
+    <row r="160" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
         <v>1</v>
       </c>
@@ -4982,8 +6051,12 @@
       <c r="G160" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="161" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P160" t="str">
+        <f t="shared" si="3"/>
+        <v>'ASROCK PHANTOM GAMING D RADEON RX 570 4G',</v>
+      </c>
+    </row>
+    <row r="161" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
         <v>1</v>
       </c>
@@ -5002,8 +6075,12 @@
       <c r="G161" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="162" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P161" t="str">
+        <f t="shared" si="3"/>
+        <v>'Tarjeta de video Gigabyte Radeon RX 570, 4GB, 256-bits',</v>
+      </c>
+    </row>
+    <row r="162" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
         <v>1</v>
       </c>
@@ -5022,8 +6099,12 @@
       <c r="G162" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="163" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P162" t="str">
+        <f t="shared" si="3"/>
+        <v>'ASROCK PHANTOM GAMING D RADEON RX 570 8G',</v>
+      </c>
+    </row>
+    <row r="163" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
         <v>1</v>
       </c>
@@ -5042,8 +6123,12 @@
       <c r="G163" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="164" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P163" t="str">
+        <f t="shared" si="3"/>
+        <v>'TARJ. VIDEO SAPPHIRE RADEON RX 570 8GB GDDR5 PULSE 256 BIT',</v>
+      </c>
+    </row>
+    <row r="164" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
         <v>1</v>
       </c>
@@ -5062,8 +6147,12 @@
       <c r="G164" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="165" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P164" t="str">
+        <f t="shared" si="3"/>
+        <v>'TARJ. VIDEO SAPPHIRE RADEON RX 5500 XT 4GB GDDR6 PULSE | 128 BIT',</v>
+      </c>
+    </row>
+    <row r="165" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
         <v>1</v>
       </c>
@@ -5082,8 +6171,12 @@
       <c r="G165" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="166" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P165" t="str">
+        <f t="shared" si="3"/>
+        <v>'ASROCK RADEON RX 5500 XT 8GB GDDR6 CHALLENGER D 8G OC | 128 BIT',</v>
+      </c>
+    </row>
+    <row r="166" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
         <v>1</v>
       </c>
@@ -5102,8 +6195,12 @@
       <c r="G166" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="167" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P166" t="str">
+        <f t="shared" si="3"/>
+        <v>'T. VIDEO GIGABYTE RADEON RX 5500 XT 4GB GDDR6',</v>
+      </c>
+    </row>
+    <row r="167" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
         <v>1</v>
       </c>
@@ -5122,8 +6219,12 @@
       <c r="G167" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="168" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P167" t="str">
+        <f t="shared" si="3"/>
+        <v>'Tarjeta de video ASUS ROG Strix AMD Radeon RX570 OC edition 8GB GDDR5 256-bit',</v>
+      </c>
+    </row>
+    <row r="168" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
         <v>1</v>
       </c>
@@ -5142,8 +6243,12 @@
       <c r="G168" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="169" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P168" t="str">
+        <f t="shared" si="3"/>
+        <v>'GIGABYTE AMD RADEON RX 580 GAMING 8GB GDDR5',</v>
+      </c>
+    </row>
+    <row r="169" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
         <v>1</v>
       </c>
@@ -5162,8 +6267,12 @@
       <c r="G169" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="170" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P169" t="str">
+        <f t="shared" si="3"/>
+        <v>'ASUS AMD ROG STRIX RX 5500XT GAMING 8GB GDDR6',</v>
+      </c>
+    </row>
+    <row r="170" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
         <v>1</v>
       </c>
@@ -5182,8 +6291,12 @@
       <c r="G170" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="171" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P170" t="str">
+        <f t="shared" si="3"/>
+        <v>'TARJETA VIDEO AMD RADEON RX 5500XT 8GB ASUS ROG STRIX GAMING',</v>
+      </c>
+    </row>
+    <row r="171" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
         <v>1</v>
       </c>
@@ -5203,7 +6316,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="172" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
         <v>1</v>
       </c>
@@ -5223,7 +6336,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="173" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
         <v>1</v>
       </c>
@@ -5243,7 +6356,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="174" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
         <v>1</v>
       </c>
@@ -5263,7 +6376,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="175" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
         <v>1</v>
       </c>
@@ -5283,7 +6396,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>472</v>
       </c>
@@ -5306,7 +6419,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
         <v>471</v>
       </c>
@@ -5326,7 +6439,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
         <v>471</v>
       </c>
@@ -5346,7 +6459,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
         <v>471</v>
       </c>
@@ -5366,7 +6479,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
         <v>471</v>
       </c>
@@ -5386,7 +6499,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
         <v>471</v>
       </c>
@@ -5406,7 +6519,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
         <v>471</v>
       </c>
@@ -5426,7 +6539,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
         <v>471</v>
       </c>
@@ -5446,7 +6559,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
         <v>471</v>
       </c>
@@ -5466,7 +6579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
         <v>471</v>
       </c>
@@ -5485,8 +6598,12 @@
       <c r="G187" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="P187" t="str">
+        <f>"'"&amp;D187&amp;"',"</f>
+        <v>'MEMORIA SODIMM T-FORCE VULCAN 8GB 3200MHZ DDR4 | RED',</v>
+      </c>
+    </row>
+    <row r="188" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
         <v>471</v>
       </c>
@@ -5505,8 +6622,12 @@
       <c r="G188" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="P188" t="str">
+        <f>"'"&amp;D188&amp;"',"</f>
+        <v>'MEMORIA DDR4 KINGSTON 8GB 3200MHZ BLACK CL16',</v>
+      </c>
+    </row>
+    <row r="189" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
         <v>471</v>
       </c>
@@ -5525,8 +6646,12 @@
       <c r="G189" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="P189" t="str">
+        <f t="shared" ref="P189:P198" si="4">"'"&amp;D189&amp;"',"</f>
+        <v>'MEMORIA HP V8SERIES 8GB 3200',</v>
+      </c>
+    </row>
+    <row r="190" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
         <v>471</v>
       </c>
@@ -5545,8 +6670,12 @@
       <c r="G190" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="P190" t="str">
+        <f t="shared" si="4"/>
+        <v>'MEM 8G HYPERX 3200GHZ DDR4',</v>
+      </c>
+    </row>
+    <row r="191" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
         <v>471</v>
       </c>
@@ -5565,8 +6694,12 @@
       <c r="G191" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="P191" t="str">
+        <f t="shared" si="4"/>
+        <v>'MEM. RAM TEAMGROUP T-FORCE DELTA DDR4 8GB/3200 NEGRO LED- RGB',</v>
+      </c>
+    </row>
+    <row r="192" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
         <v>471</v>
       </c>
@@ -5585,8 +6718,12 @@
       <c r="G192" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="193" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P192" t="str">
+        <f t="shared" si="4"/>
+        <v>'MEMORIA RAM GEIL SUPER LUCE RGB 8GB DDR4 3200MHZ',</v>
+      </c>
+    </row>
+    <row r="193" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
         <v>471</v>
       </c>
@@ -5605,8 +6742,12 @@
       <c r="G193" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="194" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P193" t="str">
+        <f t="shared" si="4"/>
+        <v>'MEM. RAM HYPERX PREDATOR RGB 8GB DDR4 3200 MHZ',</v>
+      </c>
+    </row>
+    <row r="194" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
         <v>471</v>
       </c>
@@ -5625,8 +6766,12 @@
       <c r="G194" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="195" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P194" t="str">
+        <f t="shared" si="4"/>
+        <v>'RAM T-FORCE VULCAN Z 16GB, DDR4 3200MHZ',</v>
+      </c>
+    </row>
+    <row r="195" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
         <v>471</v>
       </c>
@@ -5645,8 +6790,12 @@
       <c r="G195" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="196" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P195" t="str">
+        <f t="shared" si="4"/>
+        <v>'MEMORIA RAM KINGSTON HYPERX FURY 16GB DDR4 2666MHZ',</v>
+      </c>
+    </row>
+    <row r="196" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
         <v>471</v>
       </c>
@@ -5665,8 +6814,12 @@
       <c r="G196" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="197" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P196" t="str">
+        <f t="shared" si="4"/>
+        <v>'RAM DDR4 T-FORCE DELTA RGB 16GB 3200MHZ BLACK',</v>
+      </c>
+    </row>
+    <row r="197" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
         <v>471</v>
       </c>
@@ -5685,8 +6838,12 @@
       <c r="G197" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="198" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P197" t="str">
+        <f t="shared" si="4"/>
+        <v>'MEMORIA CORSAIR DDR4 16GB 3200MHZ VENGEANCE LPX',</v>
+      </c>
+    </row>
+    <row r="198" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
         <v>471</v>
       </c>
@@ -5705,8 +6862,12 @@
       <c r="G198" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="199" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="P198" t="str">
+        <f t="shared" si="4"/>
+        <v>'RAM KINGSTON HYPERX FURY 16GB DDR4 3200MHZ',</v>
+      </c>
+    </row>
+    <row r="199" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
         <v>471</v>
       </c>
@@ -5726,7 +6887,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="200" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
         <v>471</v>
       </c>
@@ -5746,7 +6907,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="201" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B201" t="s">
         <v>471</v>
       </c>
@@ -5766,7 +6927,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="202" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
         <v>471</v>
       </c>
@@ -5786,7 +6947,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="203" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
         <v>471</v>
       </c>
@@ -5806,7 +6967,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="204" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B204" t="s">
         <v>471</v>
       </c>
@@ -5826,7 +6987,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="205" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B205" t="s">
         <v>471</v>
       </c>
@@ -5846,7 +7007,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="206" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
         <v>471</v>
       </c>
@@ -5866,7 +7027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="207" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B207" t="s">
         <v>471</v>
       </c>
@@ -5886,7 +7047,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="208" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
         <v>471</v>
       </c>

</xml_diff>